<commit_message>
DaySaleReport Summmary Quantity/Amount tree change
</commit_message>
<xml_diff>
--- a/bin/print/ori/Summary.xlsx
+++ b/bin/print/ori/Summary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -18,11 +18,11 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Summary1" type="6" refreshedVersion="3" background="1" refreshOnLoad="1">
-    <textPr prompt="0" codePage="437" sourceFile="E:\ICS_Shaw\bin\print\Summary.txt" delimiter="|">
+  <connection id="1" name="Summary1" type="6" refreshedVersion="4" background="1" refreshOnLoad="1">
+    <textPr prompt="0" codePage="437" sourceFile="E:\ICS\bin\print\Summary.txt" tab="0" delimiter="|">
       <textFields count="15">
         <textField/>
-        <textField/>
+        <textField type="MDY"/>
         <textField/>
         <textField/>
         <textField/>
@@ -47,8 +47,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +205,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -239,6 +240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -414,14 +416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M141" sqref="M141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -436,7 +438,7 @@
     <col min="12" max="14" width="13.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -451,7 +453,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -466,7 +468,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="7"/>
@@ -482,7 +484,7 @@
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="7"/>
@@ -498,7 +500,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="7"/>
@@ -514,7 +516,7 @@
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="7"/>
@@ -530,7 +532,7 @@
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="7"/>
@@ -546,7 +548,7 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="7"/>
@@ -562,7 +564,7 @@
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="7"/>
@@ -578,7 +580,7 @@
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="7"/>
@@ -594,7 +596,7 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="7"/>
@@ -610,7 +612,7 @@
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="7"/>
@@ -626,7 +628,7 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="7"/>
@@ -642,7 +644,7 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="7"/>
@@ -658,7 +660,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="7"/>
@@ -674,7 +676,7 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="7"/>
@@ -690,7 +692,7 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="7"/>
@@ -706,7 +708,7 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
@@ -722,7 +724,7 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="7"/>
@@ -738,7 +740,7 @@
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="7"/>
@@ -754,7 +756,7 @@
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="7"/>
@@ -770,7 +772,7 @@
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="7"/>
@@ -786,7 +788,7 @@
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="7"/>
@@ -802,7 +804,7 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="7"/>
@@ -818,7 +820,7 @@
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="7"/>
@@ -834,7 +836,7 @@
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="7"/>
@@ -850,7 +852,7 @@
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="7"/>
@@ -866,7 +868,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="7"/>
@@ -882,7 +884,7 @@
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="7"/>
@@ -898,7 +900,7 @@
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="7"/>
@@ -914,7 +916,7 @@
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="7"/>
@@ -930,7 +932,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="7"/>
@@ -946,7 +948,7 @@
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="7"/>
@@ -962,7 +964,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="7"/>
@@ -978,7 +980,7 @@
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="7"/>
@@ -994,7 +996,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="7"/>
@@ -1010,7 +1012,7 @@
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="7"/>
@@ -1026,7 +1028,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="7"/>
@@ -1042,7 +1044,7 @@
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="7"/>
@@ -1058,7 +1060,7 @@
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="7"/>
@@ -1074,7 +1076,7 @@
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="7"/>
@@ -1090,7 +1092,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="7"/>
@@ -1106,7 +1108,7 @@
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="7"/>
@@ -1122,7 +1124,7 @@
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="7"/>
@@ -1138,7 +1140,7 @@
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="7"/>
@@ -1154,7 +1156,7 @@
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="7"/>
@@ -1170,7 +1172,7 @@
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="7"/>
@@ -1186,7 +1188,7 @@
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="7"/>
@@ -1202,7 +1204,7 @@
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="7"/>
@@ -1218,7 +1220,7 @@
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="7"/>
@@ -1234,7 +1236,7 @@
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="7"/>
@@ -1250,7 +1252,7 @@
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="7"/>
@@ -1266,7 +1268,7 @@
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="7"/>
@@ -1282,7 +1284,7 @@
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="7"/>
@@ -1298,7 +1300,7 @@
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="7"/>
@@ -1314,7 +1316,7 @@
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="7"/>
@@ -1330,7 +1332,7 @@
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="7"/>
@@ -1346,7 +1348,7 @@
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="7"/>
@@ -1362,7 +1364,7 @@
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="7"/>
@@ -1378,7 +1380,7 @@
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="7"/>
@@ -1394,7 +1396,7 @@
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="7"/>
@@ -1410,7 +1412,7 @@
       <c r="M61" s="7"/>
       <c r="N61" s="7"/>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="7"/>
@@ -1426,7 +1428,7 @@
       <c r="M62" s="7"/>
       <c r="N62" s="7"/>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="7"/>
@@ -1442,7 +1444,7 @@
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="7"/>
@@ -1458,7 +1460,7 @@
       <c r="M64" s="7"/>
       <c r="N64" s="7"/>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="7"/>
@@ -1474,7 +1476,7 @@
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="7"/>
@@ -1490,7 +1492,7 @@
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="7"/>
@@ -1506,7 +1508,7 @@
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="7"/>
@@ -1522,7 +1524,7 @@
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="7"/>
@@ -1538,7 +1540,7 @@
       <c r="M69" s="7"/>
       <c r="N69" s="7"/>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="7"/>
@@ -1554,7 +1556,7 @@
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="7"/>
@@ -1570,7 +1572,7 @@
       <c r="M71" s="7"/>
       <c r="N71" s="7"/>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="7"/>
@@ -1586,7 +1588,7 @@
       <c r="M72" s="7"/>
       <c r="N72" s="7"/>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="7"/>
@@ -1602,7 +1604,7 @@
       <c r="M73" s="7"/>
       <c r="N73" s="7"/>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="7"/>
@@ -1618,7 +1620,7 @@
       <c r="M74" s="7"/>
       <c r="N74" s="7"/>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="7"/>
@@ -1634,7 +1636,7 @@
       <c r="M75" s="7"/>
       <c r="N75" s="7"/>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="7"/>
@@ -1650,7 +1652,7 @@
       <c r="M76" s="7"/>
       <c r="N76" s="7"/>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="7"/>
@@ -1666,7 +1668,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="7"/>
@@ -1682,7 +1684,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="7"/>
@@ -1698,7 +1700,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="7"/>
@@ -1714,7 +1716,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="7"/>
@@ -1730,7 +1732,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="7"/>
@@ -1746,7 +1748,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="7"/>
@@ -1762,7 +1764,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="7"/>
@@ -1778,7 +1780,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="7"/>
@@ -1794,7 +1796,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="7"/>
@@ -1810,7 +1812,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="7"/>
@@ -1826,7 +1828,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="7"/>
@@ -1842,7 +1844,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="7"/>
@@ -1858,7 +1860,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="7"/>
@@ -1874,7 +1876,7 @@
       <c r="M90" s="7"/>
       <c r="N90" s="7"/>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="7"/>
@@ -1890,7 +1892,7 @@
       <c r="M91" s="7"/>
       <c r="N91" s="7"/>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="7"/>
@@ -1906,7 +1908,7 @@
       <c r="M92" s="7"/>
       <c r="N92" s="7"/>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="7"/>
@@ -1922,7 +1924,7 @@
       <c r="M93" s="7"/>
       <c r="N93" s="7"/>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="7"/>
@@ -1938,7 +1940,7 @@
       <c r="M94" s="7"/>
       <c r="N94" s="7"/>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="7"/>
@@ -1954,7 +1956,7 @@
       <c r="M95" s="7"/>
       <c r="N95" s="7"/>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="7"/>
@@ -1970,7 +1972,7 @@
       <c r="M96" s="7"/>
       <c r="N96" s="7"/>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="7"/>
@@ -1986,7 +1988,7 @@
       <c r="M97" s="7"/>
       <c r="N97" s="7"/>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="7"/>
@@ -2002,7 +2004,7 @@
       <c r="M98" s="7"/>
       <c r="N98" s="7"/>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="7"/>
@@ -2018,7 +2020,7 @@
       <c r="M99" s="7"/>
       <c r="N99" s="7"/>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="7"/>
@@ -2034,7 +2036,7 @@
       <c r="M100" s="7"/>
       <c r="N100" s="7"/>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
       <c r="C101" s="7"/>
@@ -2050,7 +2052,7 @@
       <c r="M101" s="7"/>
       <c r="N101" s="7"/>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="3"/>
       <c r="C102" s="7"/>
@@ -2066,7 +2068,7 @@
       <c r="M102" s="7"/>
       <c r="N102" s="7"/>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
       <c r="C103" s="7"/>
@@ -2082,7 +2084,7 @@
       <c r="M103" s="7"/>
       <c r="N103" s="7"/>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="7"/>
@@ -2098,7 +2100,7 @@
       <c r="M104" s="7"/>
       <c r="N104" s="7"/>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
       <c r="C105" s="7"/>
@@ -2114,7 +2116,7 @@
       <c r="M105" s="7"/>
       <c r="N105" s="7"/>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="3"/>
       <c r="C106" s="7"/>
@@ -2130,7 +2132,7 @@
       <c r="M106" s="7"/>
       <c r="N106" s="7"/>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="7"/>
@@ -2146,7 +2148,7 @@
       <c r="M107" s="7"/>
       <c r="N107" s="7"/>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="3"/>
       <c r="C108" s="7"/>
@@ -2162,7 +2164,7 @@
       <c r="M108" s="7"/>
       <c r="N108" s="7"/>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="7"/>
@@ -2178,7 +2180,7 @@
       <c r="M109" s="7"/>
       <c r="N109" s="7"/>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
       <c r="C110" s="7"/>
@@ -2194,7 +2196,7 @@
       <c r="M110" s="7"/>
       <c r="N110" s="7"/>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="7"/>
@@ -2210,7 +2212,7 @@
       <c r="M111" s="7"/>
       <c r="N111" s="7"/>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="3"/>
       <c r="C112" s="7"/>
@@ -2226,7 +2228,7 @@
       <c r="M112" s="7"/>
       <c r="N112" s="7"/>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="7"/>
@@ -2242,7 +2244,7 @@
       <c r="M113" s="7"/>
       <c r="N113" s="7"/>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="3"/>
       <c r="C114" s="7"/>
@@ -2258,7 +2260,7 @@
       <c r="M114" s="7"/>
       <c r="N114" s="7"/>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="7"/>
@@ -2274,7 +2276,7 @@
       <c r="M115" s="7"/>
       <c r="N115" s="7"/>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
       <c r="C116" s="7"/>
@@ -2290,7 +2292,7 @@
       <c r="M116" s="7"/>
       <c r="N116" s="7"/>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="7"/>
@@ -2306,7 +2308,7 @@
       <c r="M117" s="7"/>
       <c r="N117" s="7"/>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="3"/>
       <c r="C118" s="7"/>
@@ -2322,7 +2324,7 @@
       <c r="M118" s="7"/>
       <c r="N118" s="7"/>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="3"/>
       <c r="C119" s="7"/>
@@ -2338,7 +2340,7 @@
       <c r="M119" s="7"/>
       <c r="N119" s="7"/>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="3"/>
       <c r="C120" s="7"/>
@@ -2354,7 +2356,7 @@
       <c r="M120" s="7"/>
       <c r="N120" s="7"/>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
       <c r="C121" s="7"/>
@@ -2370,7 +2372,7 @@
       <c r="M121" s="7"/>
       <c r="N121" s="7"/>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="3"/>
       <c r="C122" s="7"/>
@@ -2386,7 +2388,7 @@
       <c r="M122" s="7"/>
       <c r="N122" s="7"/>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
       <c r="C123" s="7"/>
@@ -2402,7 +2404,7 @@
       <c r="M123" s="7"/>
       <c r="N123" s="7"/>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="3"/>
       <c r="C124" s="7"/>
@@ -2418,7 +2420,7 @@
       <c r="M124" s="7"/>
       <c r="N124" s="7"/>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="3"/>
       <c r="C125" s="7"/>
@@ -2434,7 +2436,7 @@
       <c r="M125" s="7"/>
       <c r="N125" s="7"/>
     </row>
-    <row r="126" spans="1:14">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="3"/>
       <c r="C126" s="7"/>
@@ -2450,7 +2452,7 @@
       <c r="M126" s="7"/>
       <c r="N126" s="7"/>
     </row>
-    <row r="127" spans="1:14">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
       <c r="C127" s="7"/>
@@ -2466,7 +2468,7 @@
       <c r="M127" s="7"/>
       <c r="N127" s="7"/>
     </row>
-    <row r="128" spans="1:14">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="3"/>
       <c r="C128" s="7"/>
@@ -2482,7 +2484,7 @@
       <c r="M128" s="7"/>
       <c r="N128" s="7"/>
     </row>
-    <row r="129" spans="1:14">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="3"/>
       <c r="C129" s="7"/>
@@ -2498,7 +2500,7 @@
       <c r="M129" s="7"/>
       <c r="N129" s="7"/>
     </row>
-    <row r="130" spans="1:14">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="3"/>
       <c r="C130" s="7"/>
@@ -2514,7 +2516,7 @@
       <c r="M130" s="7"/>
       <c r="N130" s="7"/>
     </row>
-    <row r="131" spans="1:14">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="3"/>
       <c r="C131" s="7"/>
@@ -2530,7 +2532,7 @@
       <c r="M131" s="7"/>
       <c r="N131" s="7"/>
     </row>
-    <row r="132" spans="1:14">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="3"/>
       <c r="C132" s="7"/>
@@ -2546,7 +2548,7 @@
       <c r="M132" s="7"/>
       <c r="N132" s="7"/>
     </row>
-    <row r="133" spans="1:14">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="3"/>
       <c r="C133" s="7"/>
@@ -2562,7 +2564,7 @@
       <c r="M133" s="7"/>
       <c r="N133" s="7"/>
     </row>
-    <row r="134" spans="1:14">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="3"/>
       <c r="C134" s="7"/>
@@ -2578,7 +2580,7 @@
       <c r="M134" s="7"/>
       <c r="N134" s="7"/>
     </row>
-    <row r="135" spans="1:14">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="7"/>
@@ -2594,7 +2596,7 @@
       <c r="M135" s="7"/>
       <c r="N135" s="7"/>
     </row>
-    <row r="136" spans="1:14">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="7"/>
@@ -2610,7 +2612,7 @@
       <c r="M136" s="7"/>
       <c r="N136" s="7"/>
     </row>
-    <row r="137" spans="1:14">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="3"/>
       <c r="C137" s="7"/>
@@ -2626,7 +2628,7 @@
       <c r="M137" s="7"/>
       <c r="N137" s="7"/>
     </row>
-    <row r="138" spans="1:14">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="3"/>
       <c r="C138" s="7"/>
@@ -2642,7 +2644,7 @@
       <c r="M138" s="7"/>
       <c r="N138" s="7"/>
     </row>
-    <row r="139" spans="1:14">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="3"/>
       <c r="C139" s="7"/>
@@ -2658,7 +2660,7 @@
       <c r="M139" s="7"/>
       <c r="N139" s="7"/>
     </row>
-    <row r="140" spans="1:14">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="3"/>
       <c r="C140" s="7"/>
@@ -2674,7 +2676,7 @@
       <c r="M140" s="7"/>
       <c r="N140" s="7"/>
     </row>
-    <row r="141" spans="1:14">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="3"/>
       <c r="C141" s="7"/>
@@ -2690,7 +2692,7 @@
       <c r="M141" s="7"/>
       <c r="N141" s="7"/>
     </row>
-    <row r="142" spans="1:14">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="3"/>
       <c r="C142" s="7"/>
@@ -2706,7 +2708,7 @@
       <c r="M142" s="7"/>
       <c r="N142" s="7"/>
     </row>
-    <row r="143" spans="1:14">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="3"/>
       <c r="C143" s="7"/>
@@ -2722,7 +2724,7 @@
       <c r="M143" s="7"/>
       <c r="N143" s="7"/>
     </row>
-    <row r="144" spans="1:14">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="3"/>
       <c r="C144" s="7"/>
@@ -2738,7 +2740,7 @@
       <c r="M144" s="7"/>
       <c r="N144" s="7"/>
     </row>
-    <row r="145" spans="1:14">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="3"/>
       <c r="C145" s="7"/>
@@ -2754,7 +2756,7 @@
       <c r="M145" s="7"/>
       <c r="N145" s="7"/>
     </row>
-    <row r="146" spans="1:14">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="3"/>
       <c r="C146" s="7"/>
@@ -2770,7 +2772,7 @@
       <c r="M146" s="7"/>
       <c r="N146" s="7"/>
     </row>
-    <row r="147" spans="1:14">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="7"/>
@@ -2786,7 +2788,7 @@
       <c r="M147" s="7"/>
       <c r="N147" s="7"/>
     </row>
-    <row r="148" spans="1:14">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="7"/>
@@ -2802,7 +2804,7 @@
       <c r="M148" s="7"/>
       <c r="N148" s="7"/>
     </row>
-    <row r="149" spans="1:14">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="3"/>
       <c r="C149" s="7"/>
@@ -2818,7 +2820,7 @@
       <c r="M149" s="7"/>
       <c r="N149" s="7"/>
     </row>
-    <row r="150" spans="1:14">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="3"/>
       <c r="C150" s="7"/>
@@ -2834,7 +2836,7 @@
       <c r="M150" s="7"/>
       <c r="N150" s="7"/>
     </row>
-    <row r="151" spans="1:14">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="3"/>
       <c r="C151" s="7"/>
@@ -2850,7 +2852,7 @@
       <c r="M151" s="7"/>
       <c r="N151" s="7"/>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="3"/>
       <c r="C152" s="7"/>
@@ -2866,7 +2868,7 @@
       <c r="M152" s="7"/>
       <c r="N152" s="7"/>
     </row>
-    <row r="153" spans="1:14">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="3"/>
       <c r="C153" s="7"/>
@@ -2882,7 +2884,7 @@
       <c r="M153" s="7"/>
       <c r="N153" s="7"/>
     </row>
-    <row r="154" spans="1:14">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="3"/>
       <c r="C154" s="7"/>
@@ -2898,7 +2900,7 @@
       <c r="M154" s="7"/>
       <c r="N154" s="7"/>
     </row>
-    <row r="155" spans="1:14">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="3"/>
       <c r="C155" s="7"/>
@@ -2914,7 +2916,7 @@
       <c r="M155" s="7"/>
       <c r="N155" s="7"/>
     </row>
-    <row r="156" spans="1:14">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="3"/>
       <c r="C156" s="7"/>
@@ -2930,10 +2932,10 @@
       <c r="M156" s="7"/>
       <c r="N156" s="7"/>
     </row>
-    <row r="157" spans="1:14">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B157" s="3"/>
     </row>
-    <row r="158" spans="1:14">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B158" s="3"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>

</xml_diff>